<commit_message>
msfa finance value update
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanugupta02\git\dms_Invoice_UIAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF1E176-8C83-41A8-9D1E-16D5025C08FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94077A76-B41C-416A-9139-03814ED61CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CDBA7115-E026-4056-AC8F-36C7037DED46}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="87">
   <si>
     <t>OrderId</t>
   </si>
@@ -264,13 +264,46 @@
   </si>
   <si>
     <t>Loan Rejected</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>PolicyType</t>
+  </si>
+  <si>
+    <t>PolicyNo</t>
+  </si>
+  <si>
+    <t>OldCarCustomerName</t>
+  </si>
+  <si>
+    <t>Relation</t>
+  </si>
+  <si>
+    <t>ReceiptDetails Clear</t>
+  </si>
+  <si>
+    <t>SOB15000185</t>
+  </si>
+  <si>
+    <t>123234567894</t>
+  </si>
+  <si>
+    <t>Invalid data</t>
+  </si>
+  <si>
+    <t>MSGAFinancierValue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +318,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -310,9 +350,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -320,6 +359,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,15 +677,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41155F0-825A-4766-BD15-0E5CF84D580C}">
-  <dimension ref="A1:AR5"/>
+  <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
@@ -660,25 +703,33 @@
     <col min="17" max="17" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.7265625" customWidth="1"/>
+    <col min="20" max="20" width="7.08984375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.54296875" customWidth="1"/>
+    <col min="23" max="23" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="12" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="7.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="58">
+    <row r="1" spans="1:46" ht="58">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -743,69 +794,90 @@
         <v>31</v>
       </c>
       <c r="V1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W1" t="s">
         <v>32</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>33</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>43</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>45</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>66</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>36</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>37</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>51</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>52</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>53</v>
       </c>
+      <c r="AN1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:46">
       <c r="B2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>9643785691</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1">
-        <v>123234567894</v>
+      <c r="E2" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -852,43 +924,46 @@
       <c r="U2" t="s">
         <v>61</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2">
+        <v>23</v>
+      </c>
+      <c r="W2" t="s">
         <v>38</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>39</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>60</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>5000</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>54</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>55</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:44">
+    <row r="3" spans="1:46">
       <c r="A3" t="s">
         <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>9643785691</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1">
-        <v>123234567894</v>
+      <c r="E3" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
@@ -923,10 +998,10 @@
       <c r="P3" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="R3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="S3">
@@ -938,63 +1013,66 @@
       <c r="U3" t="s">
         <v>61</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="V3">
+        <v>23</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="Y3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="4" t="s">
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AB3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="4" t="s">
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AF3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" t="s">
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" t="s">
         <v>60</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>5000</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>54</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>55</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:44">
+    <row r="4" spans="1:46">
       <c r="A4" t="s">
         <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>9643785691</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1">
-        <v>123234567894</v>
+      <c r="E4" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -1029,10 +1107,10 @@
       <c r="P4" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="R4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="S4">
@@ -1044,144 +1122,268 @@
       <c r="U4" t="s">
         <v>61</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="V4">
+        <v>23</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="Y4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="4" t="s">
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" t="s">
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" t="s">
         <v>60</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>5000</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>54</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>55</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:44">
+    <row r="5" spans="1:46">
       <c r="A5" t="s">
         <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>9643785691</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="1">
-        <v>123234567894</v>
+      <c r="E5" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
       </c>
       <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5">
+        <v>123</v>
+      </c>
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5">
+        <v>121111</v>
+      </c>
+      <c r="T5" t="s">
+        <v>13</v>
+      </c>
+      <c r="U5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V5">
+        <v>23</v>
+      </c>
+      <c r="W5" t="s">
+        <v>38</v>
+      </c>
+      <c r="X5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ5">
+        <v>5000</v>
+      </c>
+      <c r="AK5" t="s">
         <v>54</v>
       </c>
-      <c r="H5" t="s">
+      <c r="AL5" t="s">
         <v>55</v>
       </c>
-      <c r="I5" t="s">
+      <c r="AM5" t="s">
         <v>56</v>
       </c>
-      <c r="J5" t="s">
+      <c r="AN5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ5">
+        <v>12105096</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46">
+      <c r="A6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="4">
+        <v>9643785691</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K5" t="s">
+      <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L5" t="s">
+      <c r="I6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N5" t="s">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O5" t="s">
+      <c r="L6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P5" t="s">
+      <c r="M6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="N6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R5">
+      <c r="O6" s="4">
         <v>123</v>
       </c>
-      <c r="S5" t="s">
+      <c r="P6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="T5" t="s">
+      <c r="Q6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="U5" t="s">
+      <c r="R6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="V5">
+      <c r="S6" s="4">
         <v>121111</v>
       </c>
-      <c r="W5" t="s">
+      <c r="T6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="X5" t="s">
+      <c r="U6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="V6">
+        <v>23</v>
+      </c>
+      <c r="W6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="X6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AL5">
+      <c r="AJ6" s="4">
         <v>5000</v>
       </c>
-      <c r="AM5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP5">
-        <v>12105096</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>71</v>
+      <c r="AK6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN6" s="7"/>
+      <c r="AO6" s="7"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="4"/>
+      <c r="AT6" s="4"/>
+    </row>
+    <row r="7" spans="1:46">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ7">
+        <v>121050</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AN6:AO6"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>